<commit_message>
tratamento do eixo 10
</commit_message>
<xml_diff>
--- a/visao-2020/Eixo10_EstabelecimentoPrivados.xlsx
+++ b/visao-2020/Eixo10_EstabelecimentoPrivados.xlsx
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
-    <t>Sigla da UF</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -213,6 +210,9 @@
   </si>
   <si>
     <t>UF</t>
+  </si>
+  <si>
+    <t>Sigla</t>
   </si>
 </sst>
 </file>
@@ -532,47 +532,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -598,10 +596,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -627,10 +625,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -656,10 +654,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
         <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -685,10 +683,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
         <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -714,10 +712,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
         <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -743,10 +741,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
         <v>20</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -772,10 +770,10 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
         <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -801,10 +799,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
         <v>24</v>
-      </c>
-      <c r="B10" t="s">
-        <v>25</v>
       </c>
       <c r="C10">
         <v>4</v>
@@ -830,10 +828,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
         <v>26</v>
-      </c>
-      <c r="B11" t="s">
-        <v>27</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -859,10 +857,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
         <v>28</v>
-      </c>
-      <c r="B12" t="s">
-        <v>29</v>
       </c>
       <c r="C12">
         <v>6</v>
@@ -888,10 +886,10 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
         <v>30</v>
-      </c>
-      <c r="B13" t="s">
-        <v>31</v>
       </c>
       <c r="C13">
         <v>9</v>
@@ -917,10 +915,10 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
         <v>32</v>
-      </c>
-      <c r="B14" t="s">
-        <v>33</v>
       </c>
       <c r="C14">
         <v>12</v>
@@ -946,10 +944,10 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
         <v>34</v>
-      </c>
-      <c r="B15" t="s">
-        <v>35</v>
       </c>
       <c r="C15">
         <v>4</v>
@@ -975,10 +973,10 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
         <v>36</v>
-      </c>
-      <c r="B16" t="s">
-        <v>37</v>
       </c>
       <c r="C16">
         <v>3</v>
@@ -1004,10 +1002,10 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" t="s">
         <v>38</v>
-      </c>
-      <c r="B17" t="s">
-        <v>39</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -1033,10 +1031,10 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" t="s">
         <v>40</v>
-      </c>
-      <c r="B18" t="s">
-        <v>41</v>
       </c>
       <c r="C18">
         <v>6</v>
@@ -1062,10 +1060,10 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" t="s">
         <v>42</v>
-      </c>
-      <c r="B19" t="s">
-        <v>43</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -1091,10 +1089,10 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" t="s">
         <v>44</v>
-      </c>
-      <c r="B20" t="s">
-        <v>45</v>
       </c>
       <c r="C20">
         <v>6</v>
@@ -1120,10 +1118,10 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" t="s">
         <v>46</v>
-      </c>
-      <c r="B21" t="s">
-        <v>47</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -1149,10 +1147,10 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s">
         <v>48</v>
-      </c>
-      <c r="B22" t="s">
-        <v>49</v>
       </c>
       <c r="C22">
         <v>5</v>
@@ -1178,10 +1176,10 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" t="s">
         <v>50</v>
-      </c>
-      <c r="B23" t="s">
-        <v>51</v>
       </c>
       <c r="C23">
         <v>4</v>
@@ -1207,10 +1205,10 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" t="s">
         <v>52</v>
-      </c>
-      <c r="B24" t="s">
-        <v>53</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1236,10 +1234,10 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" t="s">
         <v>54</v>
-      </c>
-      <c r="B25" t="s">
-        <v>55</v>
       </c>
       <c r="C25">
         <v>4</v>
@@ -1265,10 +1263,10 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" t="s">
         <v>56</v>
-      </c>
-      <c r="B26" t="s">
-        <v>57</v>
       </c>
       <c r="C26">
         <v>19</v>
@@ -1294,10 +1292,10 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" t="s">
         <v>58</v>
-      </c>
-      <c r="B27" t="s">
-        <v>59</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1323,10 +1321,10 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" t="s">
         <v>60</v>
-      </c>
-      <c r="B28" t="s">
-        <v>61</v>
       </c>
       <c r="C28">
         <v>5</v>

</xml_diff>